<commit_message>
Rename read_ini.ini to path.ini
</commit_message>
<xml_diff>
--- a/data/pbf_case.xlsx
+++ b/data/pbf_case.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="21000" windowHeight="11790"/>
+    <workbookView windowWidth="26310" windowHeight="9480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>case_id</t>
   </si>
@@ -98,6 +98,84 @@
   </si>
   <si>
     <t>verify_null_e</t>
+  </si>
+  <si>
+    <t>tc007</t>
+  </si>
+  <si>
+    <t>创建兴趣小组成功</t>
+  </si>
+  <si>
+    <t>create_interest_group_success_p</t>
+  </si>
+  <si>
+    <t>create_interest_group_success_e</t>
+  </si>
+  <si>
+    <t>tc008</t>
+  </si>
+  <si>
+    <t>tc009</t>
+  </si>
+  <si>
+    <t>tc010</t>
+  </si>
+  <si>
+    <t>tc011</t>
+  </si>
+  <si>
+    <t>tc012</t>
+  </si>
+  <si>
+    <t>tc013</t>
+  </si>
+  <si>
+    <t>tc014</t>
+  </si>
+  <si>
+    <t>tc015</t>
+  </si>
+  <si>
+    <t>tc016</t>
+  </si>
+  <si>
+    <t>tc017</t>
+  </si>
+  <si>
+    <t>tc018</t>
+  </si>
+  <si>
+    <t>tc019</t>
+  </si>
+  <si>
+    <t>tc020</t>
+  </si>
+  <si>
+    <t>tc021</t>
+  </si>
+  <si>
+    <t>tc022</t>
+  </si>
+  <si>
+    <t>tc023</t>
+  </si>
+  <si>
+    <t>tc024</t>
+  </si>
+  <si>
+    <t>tc025</t>
+  </si>
+  <si>
+    <t>tc026</t>
+  </si>
+  <si>
+    <t>tc027</t>
+  </si>
+  <si>
+    <t>tc028</t>
+  </si>
+  <si>
+    <t>tc029</t>
   </si>
 </sst>
 </file>
@@ -733,11 +811,12 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1058,18 +1137,18 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="6" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="7.25" customWidth="1"/>
     <col min="2" max="2" width="20" customWidth="1"/>
-    <col min="3" max="3" width="16.625" customWidth="1"/>
-    <col min="4" max="4" width="16.5" customWidth="1"/>
+    <col min="3" max="3" width="29.625" customWidth="1"/>
+    <col min="4" max="4" width="29.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1169,6 +1248,196 @@
       <c r="D7" s="2" t="s">
         <v>27</v>
       </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B9" s="3"/>
+      <c r="C9" s="3"/>
+      <c r="D9" s="3"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B13" s="3"/>
+      <c r="C13" s="3"/>
+      <c r="D13" s="3"/>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
+      <c r="D17" s="3"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
+      <c r="D18" s="3"/>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B19" s="3"/>
+      <c r="C19" s="3"/>
+      <c r="D19" s="3"/>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B22" s="3"/>
+      <c r="C22" s="3"/>
+      <c r="D22" s="3"/>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>